<commit_message>
VIP Group Creation Added
</commit_message>
<xml_diff>
--- a/VIP/MyDoc.xlsx
+++ b/VIP/MyDoc.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve"> Port</t>
   </si>
   <si>
-    <t xml:space="preserve">My-VM-Name-1</t>
+    <t xml:space="preserve">My-Debian</t>
   </si>
   <si>
     <t xml:space="preserve"> 192.168.1.1</t>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">1.1.1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">My-VM-Name-2</t>
+    <t xml:space="preserve">My-CentOS</t>
   </si>
   <si>
     <t xml:space="preserve"> 192.168.1.2</t>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">1.1.1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">My-VM-Name-3</t>
+    <t xml:space="preserve">My-Ubuntu</t>
   </si>
   <si>
     <t xml:space="preserve"> 192.168.1.3</t>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">1.1.1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">My-VM-Name-4</t>
+    <t xml:space="preserve">My-FreeBSD</t>
   </si>
   <si>
     <t xml:space="preserve"> 192.168.1.4</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">1.1.1.4</t>
   </si>
   <si>
-    <t xml:space="preserve">My-VM-Name-5</t>
+    <t xml:space="preserve">My-OpenBSD</t>
   </si>
   <si>
     <t xml:space="preserve"> 192.168.1.5</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">1.1.1.5</t>
   </si>
   <si>
-    <t xml:space="preserve">My-VM-Name-6</t>
+    <t xml:space="preserve">My-laggyWin</t>
   </si>
   <si>
     <t xml:space="preserve"> 192.168.1.6</t>
@@ -186,7 +186,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -194,11 +194,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -282,7 +282,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -324,25 +324,25 @@
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="6" t="n">
         <v>80</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="6" t="n">
         <v>443</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -356,13 +356,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -373,13 +373,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -387,13 +387,13 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -404,13 +404,13 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="0" t="n">

</xml_diff>